<commit_message>
fixed error with thursday sessions
</commit_message>
<xml_diff>
--- a/src/v4.0/EGN 3310 SI with Jimmy Y. - Su22(1-15).xlsx
+++ b/src/v4.0/EGN 3310 SI with Jimmy Y. - Su22(1-15).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mynam\Documents\GitHub_Repositories\AutoGrid_Install\src\v3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mynam\Documents\GitHub_Repositories\AutoGrid\src\v4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7DD934-A632-4B3A-87AB-7C9E0B333EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502E100D-8D04-4338-AEB8-39A4D7CF6D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="375" windowWidth="26010" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -157,10 +157,19 @@
     <t>Wednesday Session 1 Hybrid</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
     <t>Eight</t>
+  </si>
+  <si>
+    <t>Monday 12:00</t>
+  </si>
+  <si>
+    <t>Monday 1:00 TCH 226</t>
+  </si>
+  <si>
+    <t>Monday 2:00 TCH 226</t>
+  </si>
+  <si>
+    <t>Monday 10:00</t>
   </si>
 </sst>
 </file>
@@ -258,8 +267,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K9" totalsRowShown="0">
-  <autoFilter ref="A1:K9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K13" totalsRowShown="0">
+  <autoFilter ref="A1:K13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="9"/>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -639,185 +648,149 @@
         <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="2"/>
       <c r="K2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44690.419687499998</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>44697.419687499998</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44697.420243055552</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2">
-        <v>44697</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
       <c r="B4" s="1">
-        <v>44697.419687499998</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44697.420243055552</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="2">
-        <v>44697</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
+        <v>44690.419687499998</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="O4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
+      <c r="A5" s="5">
+        <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>44697.445173611108</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44697.445752314823</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
+        <v>44690.419687499998</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="2">
-        <v>44697</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
+      <c r="G5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="O5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" s="5">
+        <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>44698.542048611111</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44698.543067129627</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
+        <v>44690.419687499998</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2">
-        <v>44698</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
+      <c r="G6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="O6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
+      <c r="A7" s="4">
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>44698.550127314818</v>
+        <v>44697.419687499998</v>
       </c>
       <c r="C7" s="1">
-        <v>44698.550451388888</v>
-      </c>
-      <c r="D7" t="s">
+        <v>44697.420243055552</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J7" s="2">
-        <v>44698</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
+        <v>44697</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="O7" t="s">
         <v>39</v>
@@ -825,34 +798,34 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>44699.420578703714</v>
+        <v>44697.419687499998</v>
       </c>
       <c r="C8" s="1">
-        <v>44699.421585648153</v>
+        <v>44697.420243055552</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="J8" s="2">
-        <v>44699</v>
+        <v>44697</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O8" t="s">
         <v>40</v>
@@ -860,62 +833,166 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>44699.432592592602</v>
+        <v>44697.445173611108</v>
       </c>
       <c r="C9" s="1">
-        <v>44699.433657407397</v>
+        <v>44697.445752314823</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="J9" s="2">
-        <v>44699</v>
+        <v>44697</v>
       </c>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="O9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="2"/>
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44698.542048611111</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44698.543067129627</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2">
+        <v>44698</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="2"/>
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44698.550127314818</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44698.550451388888</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2">
+        <v>44698</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="2"/>
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44699.420578703714</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44699.421585648153</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="2">
+        <v>44699</v>
+      </c>
+      <c r="K12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44699.432592592602</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44699.433657407397</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="2">
+        <v>44699</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
@@ -926,21 +1003,25 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -997,6 +1078,26 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="J33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>